<commit_message>
strat to add eu_subsidies
</commit_message>
<xml_diff>
--- a/Input_wheat.xlsx
+++ b/Input_wheat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Phil/Documents/Universität /MASTER/Decision Analysis and Forecasting for Agricultural Development/EU_Subsidies/EU_Subsidies_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F89780DE-C4A5-FB41-A05F-D468FBA683B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0DFA66-9CD8-BB4E-A796-CAF0BE65B0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5240" yWindow="6320" windowWidth="16520" windowHeight="15200" xr2:uid="{06C5D1A4-C922-2642-891E-759E2703A698}"/>
+    <workbookView xWindow="5240" yWindow="2800" windowWidth="16520" windowHeight="15200" xr2:uid="{06C5D1A4-C922-2642-891E-759E2703A698}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>variable</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>hail_insurance</t>
+  </si>
+  <si>
+    <t>eu_sub</t>
+  </si>
+  <si>
+    <t>const</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653CDCA9-EE81-1641-96D7-D446C6255374}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,6 +593,26 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>150</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>